<commit_message>
task #37 Fixed some wrong cell address and added a test with merged cell and word wrap that should not overflow
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/wrapped_text_not_overflowing.xlsx
+++ b/vaadin-spreadsheet/wrapped_text_not_overflowing.xlsx
@@ -24,12 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t xml:space="preserve">Wrap text &amp; fixed row height: Lorem ipsum dolor sit amet, no eum vitae sapientem, est eu tale accusata, ut sit scripta recusabo. Duo nullam alienum imperdiet ea, ad sit hinc mazim accusata. </t>
   </si>
   <si>
     <t>overflow control</t>
+  </si>
+  <si>
+    <t>This is a control text: this should overflow on columns B and also C since is too long and not word-wrapped</t>
+  </si>
+  <si>
+    <t>Wrapped text inside a merged cell. G2 is merged with H2 and must not overflow H2</t>
   </si>
 </sst>
 </file>
@@ -83,13 +89,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -373,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="G2" sqref="G2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -385,20 +394,24 @@
     <col min="2" max="3" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -406,8 +419,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>